<commit_message>
Recettes terminées, ID tache attribués
</commit_message>
<xml_diff>
--- a/Dossier d'architecture/Recettes.xlsx
+++ b/Dossier d'architecture/Recettes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\École\A3\Projets\Projet 2 - Prog système\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108AE340-B121-4A0A-ACD7-627DB8D20D25}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="155">
   <si>
     <t>Ingrédient requis</t>
   </si>
@@ -254,9 +255,6 @@
     <t>Semoule, raisins, concombre, poivrons</t>
   </si>
   <si>
-    <t>Préparer la semoule, couper le concombre et les poivrons et assembler le tout</t>
-  </si>
-  <si>
     <t>Huitres</t>
   </si>
   <si>
@@ -374,9 +372,6 @@
     <t>Quatre-quarts</t>
   </si>
   <si>
-    <t>Pbattez les jaunes d'œufs avec le sucre, le beurre, la farin et le blanc des œufs battus en neige. Cuire pendant 45 minutes</t>
-  </si>
-  <si>
     <t>55 minutes</t>
   </si>
   <si>
@@ -384,12 +379,123 @@
   </si>
   <si>
     <t>Œufs, beurre, sucre, farine, sel</t>
+  </si>
+  <si>
+    <t>Tarte aux pommes</t>
+  </si>
+  <si>
+    <t>Pâte brisée, pommes, sucre vanillé, beurre</t>
+  </si>
+  <si>
+    <t>Battez les jaunes d'œufs avec le sucre, le beurre, la farin et le blanc des œufs battus en neige. Cuire pendant 45 minutes</t>
+  </si>
+  <si>
+    <t>Eplucher et découper les pommes en 4 morceaux, en faire de la compote puis y ajouter le sucre. Couper les dernières pommes en fines lamelles. Verser la compote sur la pâte et les lamelles par-dessus, au four pendant 30 min</t>
+  </si>
+  <si>
+    <t>45 minutes</t>
+  </si>
+  <si>
+    <t>Moule à tarte, couteau, économe, casserole, cuillère en bois, four, fourchette, rouleau à pâtisserie</t>
+  </si>
+  <si>
+    <t>Tiramisu</t>
+  </si>
+  <si>
+    <t>Œufs, sucre roux, mascarpone, boudoir, café, cacao amer</t>
+  </si>
+  <si>
+    <t>Cuillère en bois, fouet, spatule, saladier, couvercle</t>
+  </si>
+  <si>
+    <t>Séparer les blancs des jaunes d'œufs, mélanger les jaunes avec le sucre puis ajouter le mascapone au fouet. Monter les blancs en neige et les ajouter au mélange précédent. Mettre les biscuits dans le café puis dans le plat, recouvrir de mascarpone, répéter l'opération. Saupoudrer de cacao.</t>
+  </si>
+  <si>
+    <t>Idtache</t>
+  </si>
+  <si>
+    <t>Prendre la semoule, couper le concombre et les poivrons et assembler le tout</t>
+  </si>
+  <si>
+    <t>8, 1, 3</t>
+  </si>
+  <si>
+    <t>8, 9, 8, 10</t>
+  </si>
+  <si>
+    <t>11, 15, 10, 10, 15, 3</t>
+  </si>
+  <si>
+    <t>11, 15, 15</t>
+  </si>
+  <si>
+    <t>8, 10, 15, 10</t>
+  </si>
+  <si>
+    <t>8, 10</t>
+  </si>
+  <si>
+    <t>8, 1, 3, 11, 10</t>
+  </si>
+  <si>
+    <t>8, 1</t>
+  </si>
+  <si>
+    <t>8, 23, 1, 3</t>
+  </si>
+  <si>
+    <t>8, 23, 2, 15, 3</t>
+  </si>
+  <si>
+    <t>8, 4</t>
+  </si>
+  <si>
+    <t>8, 23, 1, 5, 15, 5, 6, 15</t>
+  </si>
+  <si>
+    <t>8, 3, 15, 3, 7, 3, 10</t>
+  </si>
+  <si>
+    <t>8, 10, 11, 10</t>
+  </si>
+  <si>
+    <t>8, 10, 15</t>
+  </si>
+  <si>
+    <t>8, 23, 5, 10</t>
+  </si>
+  <si>
+    <t>8, 12</t>
+  </si>
+  <si>
+    <t>8, 23, 1, 5</t>
+  </si>
+  <si>
+    <t>8, 15</t>
+  </si>
+  <si>
+    <t>8, 13, 15, 3, 10</t>
+  </si>
+  <si>
+    <t>8, 23, 1, 15, 3, 15, 10</t>
+  </si>
+  <si>
+    <t>8, 14, 13, 7, 3, 15</t>
+  </si>
+  <si>
+    <t>8, 3, 10</t>
+  </si>
+  <si>
+    <t>8, 23, 1, 5, 15, 1, 15, 10</t>
+  </si>
+  <si>
+    <t>8, 14, 3, 7, 3, 15, 15,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -437,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -459,6 +565,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,11 +848,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -752,6 +861,7 @@
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="34.88671875" customWidth="1"/>
     <col min="5" max="6" width="23.109375" customWidth="1"/>
+    <col min="7" max="7" width="23.21875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -773,7 +883,9 @@
       <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1"/>
+      <c r="G1" s="8" t="s">
+        <v>128</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -785,7 +897,6 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -809,7 +920,9 @@
       <c r="F3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="8" t="s">
+        <v>137</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -833,7 +946,9 @@
       <c r="F4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="8" t="s">
+        <v>137</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -857,7 +972,9 @@
       <c r="F5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="8" t="s">
+        <v>138</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -881,7 +998,9 @@
       <c r="F6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="8" t="s">
+        <v>138</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -905,7 +1024,9 @@
       <c r="F7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="8" t="s">
+        <v>137</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -929,7 +1050,9 @@
       <c r="F8" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="8" t="s">
+        <v>139</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -945,7 +1068,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>76</v>
+        <v>129</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>23</v>
@@ -953,7 +1076,9 @@
       <c r="F9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -963,13 +1088,13 @@
         <v>53</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>57</v>
@@ -977,7 +1102,9 @@
       <c r="F10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="8" t="s">
+        <v>140</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -987,21 +1114,23 @@
         <v>53</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G11" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>141</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1011,21 +1140,23 @@
         <v>53</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G12" s="1"/>
+        <v>85</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1037,7 +1168,6 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1061,7 +1191,9 @@
       <c r="F14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14" s="8" t="s">
+        <v>131</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1085,7 +1217,9 @@
       <c r="F15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="1"/>
+      <c r="G15" s="8" t="s">
+        <v>132</v>
+      </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1109,7 +1243,9 @@
       <c r="F16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="1"/>
+      <c r="G16" s="8" t="s">
+        <v>133</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1133,7 +1269,9 @@
       <c r="F17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="1"/>
+      <c r="G17" s="8" t="s">
+        <v>134</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1157,7 +1295,9 @@
       <c r="F18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="1"/>
+      <c r="G18" s="8" t="s">
+        <v>135</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1181,7 +1321,9 @@
       <c r="F19" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="1"/>
+      <c r="G19" s="8" t="s">
+        <v>136</v>
+      </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1205,7 +1347,9 @@
       <c r="F20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="1"/>
+      <c r="G20" s="8" t="s">
+        <v>143</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1229,7 +1373,9 @@
       <c r="F21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G21" s="1"/>
+      <c r="G21" s="8" t="s">
+        <v>144</v>
+      </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -1253,7 +1399,9 @@
       <c r="F22" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="1"/>
+      <c r="G22" s="8" t="s">
+        <v>138</v>
+      </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -1277,7 +1425,9 @@
       <c r="F23" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="1"/>
+      <c r="G23" s="8" t="s">
+        <v>145</v>
+      </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1289,7 +1439,6 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1299,21 +1448,23 @@
         <v>67</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G25" s="1"/>
+      <c r="G25" s="8" t="s">
+        <v>146</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1323,21 +1474,23 @@
         <v>67</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>57</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G26" s="1"/>
+        <v>94</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>147</v>
+      </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1347,13 +1500,13 @@
         <v>67</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>46</v>
@@ -1361,7 +1514,9 @@
       <c r="F27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="1"/>
+      <c r="G27" s="8" t="s">
+        <v>138</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1371,19 +1526,21 @@
         <v>67</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="F28" s="3"/>
-      <c r="G28" s="1"/>
+      <c r="G28" s="8" t="s">
+        <v>148</v>
+      </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -1393,21 +1550,23 @@
         <v>67</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E29" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G29" s="1"/>
+      <c r="G29" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -1417,21 +1576,23 @@
         <v>67</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="G30" s="1"/>
+        <v>108</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -1441,21 +1602,23 @@
         <v>67</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="G31" s="1"/>
+      <c r="G31" s="8" t="s">
+        <v>151</v>
+      </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -1465,49 +1628,75 @@
         <v>67</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D32" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G32" s="1"/>
+      <c r="G32" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="1"/>
+      <c r="B33" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>153</v>
+      </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="1"/>
+      <c r="B34" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>154</v>
+      </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -1519,7 +1708,6 @@
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -1530,7 +1718,6 @@
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -1541,7 +1728,6 @@
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -1552,7 +1738,6 @@
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -1563,7 +1748,6 @@
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -1574,7 +1758,6 @@
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -1585,7 +1768,6 @@
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
@@ -1596,7 +1778,6 @@
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -1607,7 +1788,6 @@
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -1618,7 +1798,6 @@
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -1629,7 +1808,6 @@
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -1641,7 +1819,6 @@
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
@@ -1653,7 +1830,6 @@
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>

</xml_diff>